<commit_message>
Refactor keyword classification prompts and output format
- Updated system prompt to clarify classification criteria for appliance repair terms, including new device scope and geographic rules.
- Changed user prompt format from JSON array to a comma-separated list for easier input processing.
- Revised AI output sample to align with new explanation format and classification rules.
- Added new user prompt and output sample files for additional test cases, ensuring comprehensive coverage of classification scenarios.
</commit_message>
<xml_diff>
--- a/gelismis_output.xlsx
+++ b/gelismis_output.xlsx
@@ -8,9 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Veri Raporu" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="30_Keywords_Report" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="50_Keywords_Report" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Veri Raporu'!$A$1:$E$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'30_Keywords_Report'!$A$1:$E$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'50_Keywords_Report'!$A$1:$E$51</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1180,4 +1184,1952 @@
   <autoFilter ref="A1:E31"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="80" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>is_positive</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>match_type</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>explanation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>altus servis</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>beyaz eşya tamircileri</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>[Accept reason: Contains strong repair intent]. [Match type reasoning: Clearly repair-related phrase with flexibility].</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>buzdolabı</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Lacks clear service intent]. [Match type reasoning: Generic term without repair action].</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>nebiler baymak servis</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>vestel çamaşır makinesi</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Brand reference implies official service].</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>sharp buzdolabı servisi</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Brand reference implies official service].</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>camasir makinesi servisi</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>[Accept reason: Contains strong repair intent]. [Match type reasoning: Clearly repair-related phrase].</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>çamaşır makinesi tesisatı</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Focuses on installation]. [Match type reasoning: Lacks clear repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>alibeyköy buzdolabı tamircisi</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>exact</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>[Accept reason: Contains strong service intent and specific location]. [Match type reasoning: Exact match due to specific location and repair action].</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>leısure servis</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>arnavutköy çamaşır makinesi tamir</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>exact</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>[Accept reason: Contains strong service intent and specific location]. [Match type reasoning: Exact match due to specific location and repair action].</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1">
+      <c r="A13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>arçelik servis</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>bursa çamaşır makinesi tamiri</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>samsung çamaşır makinesi tamircisi</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>[Accept reason: Contains strong repair intent]. [Match type reasoning: Brand reference implies third-party repair].</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>televizyon tamir</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>[Accept reason: Contains strong repair intent]. [Match type reasoning: Clearly repair-related phrase].</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>demirdöküm servis</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>ferroli kombi servis</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Brand reference implies official service].</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="30" customHeight="1">
+      <c r="A19" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>airfel kombi servis bandırma</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="30" customHeight="1">
+      <c r="A20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>görükle televizyon tamircisi</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="30" customHeight="1">
+      <c r="A21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>profilo servis numarası</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Requests contact info]. [Match type reasoning: Lacks clear service intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>teknikel servis</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>kartepe beyaz eşya tamircisi</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>klima iç ünite</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Focuses on components]. [Match type reasoning: Lacks clear repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="30" customHeight="1">
+      <c r="A25" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>sanko oto klima</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Refers to a device outside the supported scope]. [Match type reasoning: Lacks clear repair intent].</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="30" customHeight="1">
+      <c r="A26" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>söke klima tamircisi</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="30" customHeight="1">
+      <c r="A27" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>klima servisi aydın</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="30" customHeight="1">
+      <c r="A28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>sigma klima servis izmir</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="30" customHeight="1">
+      <c r="A29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>silifke klima tamircileri</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Specifies a city outside Istanbul]. [Match type reasoning: Lacks relevance to Istanbul].</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="30" customHeight="1">
+      <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>york klima</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Lacks clear service intent]. [Match type reasoning: Generic term without repair action].</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="30" customHeight="1">
+      <c r="A31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>bosch servisi</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>[Reject reason: Mentions official service]. [Match type reasoning: Generic term without strong repair intent].</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E31"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="80" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>is_positive</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>match_type</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>explanation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>en yakın klima servisi</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for klima in Istanbul]. [Phrase match as it indicates a nearby service search.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>beko çamaşır makinesi teknik servis</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>en yakın beyaz eşya tamircisi</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for beyaz eşya in Istanbul]. [Phrase match as it indicates a nearby repair service search.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>airfel kombi servis numarası</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to request for contact information]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>görükle tv tamircisi</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>exact</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for TV in Görükle, Istanbul]. [Exact match as it specifies a location and repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>trabzon buzdolabı tamircisi</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to specifying a city outside Istanbul]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>akçaabat arçelik servisi</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>vestel servis</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>altus buzdolabı servis</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>demirdöküm servis</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>arçelik servis</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1">
+      <c r="A13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>bosch un telefon numarası</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to request for contact information]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>keysmart buzdolabı servisi</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>görükle çamaşır makinesi tamiri</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>exact</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for çamaşır makinesi in Görükle, Istanbul]. [Exact match as it specifies a location and repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>arçelik buzdolabı servis</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>altus klima bakımı</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to focusing on maintenance rather than repair]. [Broad match as it lacks repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>grundig servis</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="30" customHeight="1">
+      <c r="A19" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>sigma klima fa arızası</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for klima with fault indication]. [Phrase match as it indicates a repair issue.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="30" customHeight="1">
+      <c r="A20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>dijitsu klima servis</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="30" customHeight="1">
+      <c r="A21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>arçelik klima tespit</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to focusing on diagnostics rather than repair]. [Broad match as it lacks repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>hoover çamaşır makinesi servis numarası</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to request for contact information]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>klima servis</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to being vague and lacking specific repair intent]. [Broad match as it lacks repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>pursaklar buzdolabı tamircisi</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>exact</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for buzdolabı in Pursaklar, Istanbul]. [Exact match as it specifies a location and repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="30" customHeight="1">
+      <c r="A25" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>buzdolabı tamircisi ankara mamak</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to specifying a city outside Istanbul]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="30" customHeight="1">
+      <c r="A26" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>kombi tamircisi</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for kombi]. [Broad match as it indicates a general repair service.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="30" customHeight="1">
+      <c r="A27" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>3m servis üçkuyular</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="30" customHeight="1">
+      <c r="A28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>balıkesir klima servisi</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to specifying a city outside Istanbul]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="30" customHeight="1">
+      <c r="A29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>eryaman klima servisi</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to specifying a city outside Istanbul]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="30" customHeight="1">
+      <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>baymak servisi karataş</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="30" customHeight="1">
+      <c r="A31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>tomalar vaillant servisi</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>demirdöküm servisi güvenlik</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="30" customHeight="1">
+      <c r="A33" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>kanal vaillant servisi</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="30" customHeight="1">
+      <c r="A34" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>gemlik demirdöküm servis</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to specifying a city outside Istanbul]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="30" customHeight="1">
+      <c r="A35" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>kılınçarslan baymak servisi</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E35" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="30" customHeight="1">
+      <c r="A36" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>söke klima tamircisi</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to specifying a city outside Istanbul]. [Broad match as it lacks repair action and is location-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="30" customHeight="1">
+      <c r="A37" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>pendik kombi</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>exact</t>
+        </is>
+      </c>
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for kombi in Pendik, Istanbul]. [Exact match as it specifies a location and repair action.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="30" customHeight="1">
+      <c r="A38" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>ferroli kombi f arıza kodu</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for kombi with fault indication]. [Phrase match as it indicates a repair issue.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="30" customHeight="1">
+      <c r="A39" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>altus teknik servis</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="30" customHeight="1">
+      <c r="A40" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>şanlıurfa regal servis numarası</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to request for contact information]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="30" customHeight="1">
+      <c r="A41" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>kombi servisi</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for kombi]. [Broad match as it indicates a general repair service.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="30" customHeight="1">
+      <c r="A42" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>bulaşık makinesi yıkamadan bitiyor</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for bulaşık makinesi with fault indication]. [Phrase match as it indicates a repair issue.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="30" customHeight="1">
+      <c r="A43" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>balıkesir bosch servisi telefon numarası</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to request for contact information]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="30" customHeight="1">
+      <c r="A44" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>demetevler baymak kombi servisi</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="30" customHeight="1">
+      <c r="A45" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>iklimsa edremit servis</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="30" customHeight="1">
+      <c r="A46" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>karaveliler demirdöküm servis</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="30" customHeight="1">
+      <c r="A47" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>sarısu vaillant servis</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to official service seeking intent]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="30" customHeight="1">
+      <c r="A48" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>hotpoint ariston servis numarası</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to request for contact information]. [Broad match as it lacks repair action and is brand-specific.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="30" customHeight="1">
+      <c r="A49" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>beyaz eşya tamirhanesi</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for beyaz eşya]. [Broad match as it indicates a general repair service.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="30" customHeight="1">
+      <c r="A50" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>electrolux çamaşır makinesi arızaları</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>phrase</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>[Accepted due to clear repair intent for çamaşır makinesi with fault indication]. [Phrase match as it indicates a repair issue.]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="30" customHeight="1">
+      <c r="A51" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>ay teknik çekmekoy</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>broad</t>
+        </is>
+      </c>
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>[Rejected due to being vague and lacking specific repair intent]. [Broad match as it lacks repair action.]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E51"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>